<commit_message>
remove some column not use
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/BaoCao/Teamplate_NhatKySuDungDichVu_TheGiaTri.xlsx
+++ b/banhang24/Template/ExportExcel/BaoCao/Teamplate_NhatKySuDungDichVu_TheGiaTri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\banhang24_20180625\banhang24vn\banhang24\Template\ExportExcel\BaoCao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\KangJinDemo\KangJinDemo\banhang24\Template\ExportExcel\BaoCao\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Thời gian:</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tổng: </t>
+  </si>
+  <si>
+    <t>Phát sinh tăng</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -303,6 +306,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -585,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,17 +605,17 @@
     <col min="4" max="4" width="22.140625" style="14" customWidth="1"/>
     <col min="5" max="5" width="22" style="14" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" style="28" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="26" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" style="26" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="2"/>
+    <col min="7" max="8" width="18.7109375" style="28" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="26" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>3</v>
       </c>
@@ -625,22 +631,24 @@
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
       <c r="M1" s="31"/>
-    </row>
-    <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="N1" s="31"/>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="15"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
       <c r="G2" s="18"/>
-      <c r="H2" s="23"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="23"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="18"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="18"/>
-      <c r="M2" s="16"/>
-    </row>
-    <row r="3" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="M2" s="18"/>
+      <c r="N2" s="16"/>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>0</v>
       </c>
@@ -650,19 +658,20 @@
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="23"/>
+      <c r="H3" s="18"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="17"/>
       <c r="L3" s="18"/>
-      <c r="M3" s="16"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3" s="18"/>
+      <c r="N3" s="16"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -684,26 +693,29 @@
       <c r="G6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="J6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="M6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="N6" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="6"/>
       <c r="C7" s="24"/>
@@ -711,14 +723,15 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="7"/>
       <c r="I7" s="24"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="24"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="19"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="7"/>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6"/>
       <c r="C8" s="24"/>
@@ -726,14 +739,15 @@
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="7"/>
       <c r="I8" s="24"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="24"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8" s="19"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="7"/>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="6"/>
       <c r="C9" s="24"/>
@@ -741,14 +755,15 @@
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="24"/>
-      <c r="J9" s="7"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="19"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M9" s="7"/>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="24"/>
@@ -756,14 +771,15 @@
       <c r="E10" s="24"/>
       <c r="F10" s="24"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="24"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="24"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="7"/>
+      <c r="N10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="24"/>
@@ -771,14 +787,15 @@
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
-      <c r="M11" s="19"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="7"/>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="24"/>
@@ -786,14 +803,15 @@
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="24"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
-      <c r="M12" s="19"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M12" s="7"/>
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="24"/>
@@ -801,14 +819,15 @@
       <c r="E13" s="24"/>
       <c r="F13" s="24"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="7"/>
       <c r="I13" s="24"/>
-      <c r="J13" s="7"/>
+      <c r="J13" s="24"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
-      <c r="M13" s="19"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="7"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
       <c r="C14" s="24"/>
@@ -816,14 +835,15 @@
       <c r="E14" s="24"/>
       <c r="F14" s="24"/>
       <c r="G14" s="7"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="24"/>
-      <c r="J14" s="7"/>
+      <c r="J14" s="24"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="7"/>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="6"/>
       <c r="C15" s="24"/>
@@ -831,14 +851,15 @@
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="7"/>
       <c r="I15" s="24"/>
-      <c r="J15" s="7"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M15" s="7"/>
+      <c r="N15" s="19"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="6"/>
       <c r="C16" s="24"/>
@@ -846,14 +867,15 @@
       <c r="E16" s="24"/>
       <c r="F16" s="24"/>
       <c r="G16" s="7"/>
-      <c r="H16" s="24"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="24"/>
-      <c r="J16" s="7"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="19"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M16" s="7"/>
+      <c r="N16" s="19"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="6"/>
       <c r="C17" s="24"/>
@@ -861,14 +883,15 @@
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="24"/>
-      <c r="J17" s="7"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="19"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="7"/>
+      <c r="N17" s="19"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="6"/>
       <c r="C18" s="24"/>
@@ -876,14 +899,15 @@
       <c r="E18" s="24"/>
       <c r="F18" s="24"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="24"/>
+      <c r="H18" s="7"/>
       <c r="I18" s="24"/>
-      <c r="J18" s="7"/>
+      <c r="J18" s="24"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="19"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M18" s="7"/>
+      <c r="N18" s="19"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="6"/>
       <c r="C19" s="24"/>
@@ -891,14 +915,15 @@
       <c r="E19" s="24"/>
       <c r="F19" s="24"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="24"/>
+      <c r="H19" s="7"/>
       <c r="I19" s="24"/>
-      <c r="J19" s="7"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="19"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="7"/>
+      <c r="N19" s="19"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="6"/>
       <c r="C20" s="24"/>
@@ -906,14 +931,15 @@
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="24"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="24"/>
-      <c r="J20" s="7"/>
+      <c r="J20" s="24"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M20" s="7"/>
+      <c r="N20" s="19"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="6"/>
       <c r="C21" s="24"/>
@@ -921,14 +947,15 @@
       <c r="E21" s="24"/>
       <c r="F21" s="24"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="24"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="24"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
-      <c r="M21" s="19"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M21" s="7"/>
+      <c r="N21" s="19"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="6"/>
       <c r="C22" s="24"/>
@@ -936,14 +963,15 @@
       <c r="E22" s="24"/>
       <c r="F22" s="24"/>
       <c r="G22" s="7"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="7"/>
       <c r="I22" s="24"/>
-      <c r="J22" s="7"/>
+      <c r="J22" s="24"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
-      <c r="M22" s="19"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M22" s="7"/>
+      <c r="N22" s="19"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="6"/>
       <c r="C23" s="24"/>
@@ -951,14 +979,15 @@
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="24"/>
-      <c r="J23" s="7"/>
+      <c r="J23" s="24"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
-      <c r="M23" s="19"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23" s="7"/>
+      <c r="N23" s="19"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="6"/>
       <c r="C24" s="24"/>
@@ -966,14 +995,15 @@
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
       <c r="G24" s="7"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="24"/>
-      <c r="J24" s="7"/>
+      <c r="J24" s="24"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
-      <c r="M24" s="19"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="7"/>
+      <c r="N24" s="19"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="6"/>
       <c r="C25" s="24"/>
@@ -981,14 +1011,15 @@
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="7"/>
       <c r="I25" s="24"/>
-      <c r="J25" s="7"/>
+      <c r="J25" s="24"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
-      <c r="M25" s="19"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M25" s="7"/>
+      <c r="N25" s="19"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="6"/>
       <c r="C26" s="24"/>
@@ -996,14 +1027,15 @@
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="7"/>
       <c r="I26" s="24"/>
-      <c r="J26" s="7"/>
+      <c r="J26" s="24"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
-      <c r="M26" s="19"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="7"/>
+      <c r="N26" s="19"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="6"/>
       <c r="C27" s="24"/>
@@ -1011,14 +1043,15 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="7"/>
       <c r="I27" s="24"/>
-      <c r="J27" s="7"/>
+      <c r="J27" s="24"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="M27" s="19"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M27" s="7"/>
+      <c r="N27" s="19"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="6"/>
       <c r="C28" s="24"/>
@@ -1026,14 +1059,15 @@
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="24"/>
-      <c r="J28" s="7"/>
+      <c r="J28" s="24"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
-      <c r="M28" s="19"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M28" s="7"/>
+      <c r="N28" s="19"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="6"/>
       <c r="C29" s="24"/>
@@ -1041,14 +1075,15 @@
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="24"/>
-      <c r="J29" s="7"/>
+      <c r="J29" s="24"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
-      <c r="M29" s="19"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M29" s="7"/>
+      <c r="N29" s="19"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="6"/>
       <c r="C30" s="24"/>
@@ -1056,14 +1091,15 @@
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="24"/>
-      <c r="J30" s="7"/>
+      <c r="J30" s="24"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
-      <c r="M30" s="19"/>
-    </row>
-    <row r="31" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M30" s="7"/>
+      <c r="N30" s="19"/>
+    </row>
+    <row r="31" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
         <v>16</v>
       </c>
@@ -1079,16 +1115,17 @@
         <f xml:space="preserve"> SUM(G7:G$30)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="25"/>
+      <c r="H31" s="32"/>
       <c r="I31" s="25"/>
-      <c r="J31" s="21"/>
+      <c r="J31" s="25"/>
       <c r="K31" s="21"/>
       <c r="L31" s="21"/>
-      <c r="M31" s="22"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
- add column {MaNhanVien, TenNhanVien}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/BaoCao/Teamplate_NhatKySuDungDichVu_TheGiaTri.xlsx
+++ b/banhang24/Template/ExportExcel/BaoCao/Teamplate_NhatKySuDungDichVu_TheGiaTri.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Thời gian:</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>Phát sinh tăng</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>Tên nhân viên</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -259,27 +265,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -304,11 +301,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -591,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,73 +617,79 @@
     <col min="4" max="4" width="22.140625" style="14" customWidth="1"/>
     <col min="5" max="5" width="22" style="14" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" style="14" customWidth="1"/>
-    <col min="7" max="8" width="18.7109375" style="28" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="26" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="26" customWidth="1"/>
+    <col min="7" max="8" width="18.7109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="23" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="23" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" style="4" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="13" max="15" width="16.28515625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" style="31" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:16" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+    </row>
+    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="15"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="16"/>
-    </row>
-    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="30"/>
+    </row>
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="16"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="30"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="5" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -714,418 +732,474 @@
       <c r="N6" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="6"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="19"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="33"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="6"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-      <c r="N8" s="19"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="33"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="19"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="33"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="6"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-      <c r="N10" s="19"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="33"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="19"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="33"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="19"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="33"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="19"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="33"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
-      <c r="N14" s="19"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="33"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
-      <c r="N15" s="19"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="33"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="6"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="19"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="33"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="19"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="33"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="19"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="33"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="19"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="33"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
       <c r="K20" s="7"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
-      <c r="N20" s="19"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="33"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="21"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="19"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="33"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="19"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="33"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="6"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
-      <c r="N23" s="19"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="33"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
-      <c r="N24" s="19"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="33"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="19"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="33"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
       <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="19"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="33"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
-      <c r="N27" s="19"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="33"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="19"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="33"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="6"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
       <c r="K29" s="7"/>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="19"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="33"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
       <c r="K30" s="7"/>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="19"/>
-    </row>
-    <row r="31" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="33"/>
+    </row>
+    <row r="31" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="27">
+      <c r="B31" s="19"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="24">
         <f xml:space="preserve"> SUM(F7:F$30)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="26">
         <f xml:space="preserve"> SUM(G7:G$30)</f>
         <v>0</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="22"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>